<commit_message>
- add list column for 'NhapKhoNoiBo'
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Download/0973474985/28fef5a1-f0f2-4b94-a4ad-081b227f3b77/PhieuNhapHang.xlsx
+++ b/banhang24/Template/ExportExcel/Download/0973474985/28fef5a1-f0f2-4b94-a4ad-081b227f3b77/PhieuNhapHang.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Ghi chú</t>
   </si>
@@ -25,18 +25,36 @@
     <t>Tổng tiền hàng</t>
   </si>
   <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
     <t>DANH SÁCH TỔNG HỢP PHIẾU NHẬP HÀNG</t>
   </si>
   <si>
+    <t>Cần trả NCC</t>
+  </si>
+  <si>
     <t>Đã trả NCC</t>
   </si>
   <si>
     <t>Mã NCC</t>
   </si>
   <si>
+    <t>Tên NCC</t>
+  </si>
+  <si>
     <t>Số điện thoại</t>
   </si>
   <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>NV lập HĐ</t>
+  </si>
+  <si>
+    <t>Tổng giảm giá</t>
+  </si>
+  <si>
     <t>Tổng tiền thuế</t>
   </si>
   <si>
@@ -46,6 +64,9 @@
     <t>Ngày lập hóa đơn</t>
   </si>
   <si>
+    <t>Tên chi nhánh</t>
+  </si>
+  <si>
     <t>Còn nợ</t>
   </si>
   <si>
@@ -61,44 +82,56 @@
     <t>Tiền POS</t>
   </si>
   <si>
+    <t>Tổng tiền trước CK</t>
+  </si>
+  <si>
     <t>Tổng chiết khấu</t>
   </si>
   <si>
-    <t>CG.01_PNK2022060804</t>
-  </si>
-  <si>
-    <t>NCC000043</t>
+    <t>CG.01__PNK2206.04</t>
+  </si>
+  <si>
+    <t>NCCL001</t>
+  </si>
+  <si>
+    <t>Nhà Cung Cấp Lẻ</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>nhapmua from po
-nợ: 100K</t>
-  </si>
-  <si>
-    <t>CG.01_PNK2022060803</t>
+    <t>CG_NV2909_01</t>
+  </si>
+  <si>
+    <t>Ssoft CN Cầu Giấy</t>
+  </si>
+  <si>
+    <t>nhap noi bo - menu rieng</t>
+  </si>
+  <si>
+    <t>Đã nhập hàng</t>
+  </si>
+  <si>
+    <t>CG.01__PNK2206.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đào Thị Long Lanh Kim Ánh Dương </t>
+  </si>
+  <si>
+    <t>check nóiungthuchi = makhach + ten
+khoanthuchi = chi nhapnoibo</t>
+  </si>
+  <si>
+    <t>CG.01__PNK2206.01</t>
   </si>
   <si>
     <t>NCC000228</t>
   </si>
   <si>
-    <t>nhapmua - lan 2 (het)</t>
-  </si>
-  <si>
-    <t>CG.01_PNK2022060802</t>
-  </si>
-  <si>
-    <t>nhapmua from PO</t>
-  </si>
-  <si>
-    <t>CG.01_PNK2022060702</t>
-  </si>
-  <si>
-    <t>NCCL001</t>
-  </si>
-  <si>
-    <t>CG.01_PNK2022060701</t>
+    <t>NCC xe cu</t>
+  </si>
+  <si>
+    <t>update lan 2 - nhieu dvt - check tonkho</t>
   </si>
 </sst>
 </file>
@@ -706,7 +739,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -719,19 +752,27 @@
     <col min="1" max="1" width="23.5714285714286" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.4285714285714" style="13" customWidth="1"/>
     <col min="3" max="3" width="19.4285714285714" style="13" customWidth="1"/>
-    <col min="4" max="4" width="22.2857142857143" style="8" customWidth="1"/>
-    <col min="5" max="5" width="21.7142857142857" style="22" customWidth="1"/>
-    <col min="6" max="7" width="19.7142857142857" style="22" customWidth="1"/>
-    <col min="8" max="11" width="18.1428571428571" style="22" customWidth="1"/>
-    <col min="12" max="12" width="21.7142857142857" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.7142857142857" style="22" customWidth="1"/>
-    <col min="14" max="14" width="21.7142857142857" style="11" customWidth="1"/>
-    <col min="15" max="16384" width="9.14285714285714" style="1"/>
+    <col min="4" max="4" width="31.1428571428571" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.2857142857143" style="8" customWidth="1"/>
+    <col min="6" max="6" width="31.1428571428571" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.2857142857143" style="8" customWidth="1"/>
+    <col min="8" max="8" width="18.1428571428571" style="6" customWidth="1"/>
+    <col min="9" max="9" width="23.4285714285714" style="22" customWidth="1"/>
+    <col min="10" max="10" width="21.7142857142857" style="22" customWidth="1"/>
+    <col min="11" max="12" width="19.7142857142857" style="22" customWidth="1"/>
+    <col min="13" max="13" width="19.1428571428571" style="22" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1428571428571" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="18.1428571428571" style="22" customWidth="1"/>
+    <col min="19" max="19" width="21.7142857142857" style="22" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.7142857142857" style="22" customWidth="1"/>
+    <col min="21" max="21" width="21.7142857142857" style="11" customWidth="1"/>
+    <col min="22" max="22" width="17.8571428571429" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="27.75" customHeight="1">
+    <row r="1" spans="1:22" ht="27.75" customHeight="1">
       <c r="A1" s="30" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -744,322 +785,349 @@
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="19"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="5"/>
     </row>
     <row r="2" ht="15">
       <c r="A2" s="1"/>
     </row>
-    <row r="4" spans="1:14" s="7" customFormat="1" ht="25.5" customHeight="1">
+    <row r="4" spans="1:22" s="7" customFormat="1" ht="25.5" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="E4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="F4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="O4" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>0</v>
+      <c r="T4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15">
+    <row r="5" spans="1:22" ht="15">
       <c r="A5" s="15" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B5" s="16">
-        <v>44720.6108101852</v>
+        <v>44725.7476851852</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="31">
-        <v>239000</v>
-      </c>
-      <c r="F5" s="21">
-        <v>2151000</v>
-      </c>
-      <c r="G5" s="21">
-        <v>0</v>
-      </c>
-      <c r="H5" s="21">
-        <v>1551000</v>
-      </c>
-      <c r="I5" s="21">
-        <v>500000</v>
-      </c>
-      <c r="J5" s="21">
+        <v>25</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="31">
+        <v>2116000</v>
+      </c>
+      <c r="J5" s="31">
         <v>0</v>
       </c>
       <c r="K5" s="21">
-        <v>0</v>
+        <v>2116000</v>
       </c>
       <c r="L5" s="21">
-        <v>2051000</v>
+        <v>0</v>
       </c>
       <c r="M5" s="21">
-        <v>100000</v>
-      </c>
-      <c r="N5" s="12" t="s">
-        <v>18</v>
+        <v>0</v>
+      </c>
+      <c r="N5" s="21">
+        <v>2116000</v>
+      </c>
+      <c r="O5" s="21">
+        <v>0</v>
+      </c>
+      <c r="P5" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>0</v>
+      </c>
+      <c r="R5" s="21">
+        <v>0</v>
+      </c>
+      <c r="S5" s="21">
+        <v>0</v>
+      </c>
+      <c r="T5" s="21">
+        <v>2116000</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="V5" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15">
+    <row r="6" spans="1:22" ht="15">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B6" s="16">
-        <v>44720.5008912037</v>
+        <v>44725.6558101852</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="31">
-        <v>0</v>
-      </c>
-      <c r="F6" s="21">
-        <v>120000</v>
-      </c>
-      <c r="G6" s="21">
-        <v>0</v>
-      </c>
-      <c r="H6" s="21">
-        <v>120000</v>
-      </c>
-      <c r="I6" s="21">
-        <v>0</v>
-      </c>
-      <c r="J6" s="21">
+        <v>25</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="31">
+        <v>405000</v>
+      </c>
+      <c r="J6" s="31">
         <v>0</v>
       </c>
       <c r="K6" s="21">
-        <v>0</v>
+        <v>405000</v>
       </c>
       <c r="L6" s="21">
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="M6" s="21">
         <v>0</v>
       </c>
-      <c r="N6" s="12" t="s">
-        <v>21</v>
+      <c r="N6" s="21">
+        <v>405000</v>
+      </c>
+      <c r="O6" s="21">
+        <v>400000</v>
+      </c>
+      <c r="P6" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>0</v>
+      </c>
+      <c r="R6" s="21">
+        <v>0</v>
+      </c>
+      <c r="S6" s="21">
+        <v>400000</v>
+      </c>
+      <c r="T6" s="21">
+        <v>5000</v>
+      </c>
+      <c r="U6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="V6" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:22" ht="15">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B7" s="16">
-        <v>44720.4995949074</v>
+        <v>44723.404212963</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="31">
-        <v>0</v>
-      </c>
-      <c r="F7" s="21">
-        <v>30000</v>
-      </c>
-      <c r="G7" s="21">
-        <v>0</v>
-      </c>
-      <c r="H7" s="21">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21">
-        <v>30000</v>
-      </c>
-      <c r="J7" s="21">
+        <v>36</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0</v>
+      </c>
+      <c r="J7" s="31">
         <v>0</v>
       </c>
       <c r="K7" s="21">
         <v>0</v>
       </c>
       <c r="L7" s="21">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="M7" s="21">
         <v>0</v>
       </c>
-      <c r="N7" s="12" t="s">
-        <v>23</v>
+      <c r="N7" s="21">
+        <v>0</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0</v>
+      </c>
+      <c r="P7" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>0</v>
+      </c>
+      <c r="R7" s="21">
+        <v>0</v>
+      </c>
+      <c r="S7" s="21">
+        <v>0</v>
+      </c>
+      <c r="T7" s="21">
+        <v>0</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="18" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="16">
-        <v>44719.7189930556</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="31">
-        <v>0</v>
-      </c>
-      <c r="F8" s="21">
-        <v>500000</v>
-      </c>
-      <c r="G8" s="21">
-        <v>0</v>
-      </c>
-      <c r="H8" s="21">
-        <v>0</v>
-      </c>
-      <c r="I8" s="21">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21">
-        <v>0</v>
-      </c>
-      <c r="K8" s="21">
-        <v>0</v>
-      </c>
-      <c r="L8" s="21">
-        <v>0</v>
-      </c>
-      <c r="M8" s="21">
-        <v>500000</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15">
-      <c r="A9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="16">
-        <v>44719.6580439815</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="31">
-        <v>0</v>
-      </c>
-      <c r="F9" s="21">
-        <v>2500000</v>
-      </c>
-      <c r="G9" s="21">
-        <v>0</v>
-      </c>
-      <c r="H9" s="21">
-        <v>0</v>
-      </c>
-      <c r="I9" s="21">
-        <v>0</v>
-      </c>
-      <c r="J9" s="21">
-        <v>0</v>
-      </c>
-      <c r="K9" s="21">
-        <v>0</v>
-      </c>
-      <c r="L9" s="21">
-        <v>0</v>
-      </c>
-      <c r="M9" s="21">
-        <v>2500000</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="23.25" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="29">
-        <f>SUM(E$5:E9)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="29">
-        <f>SUM(F$5:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="29">
-        <f>SUM(G$5:G9)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="29">
-        <f>SUM(H$5:H9)</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="29">
-        <f>SUM(I$5:I9)</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="29">
-        <f>SUM(J$5:J9)</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="29">
-        <f>SUM(K$5:K9)</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="29">
-        <f>SUM(L$5:L9)</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="29">
-        <f>SUM(M$5:M9)</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="26"/>
+    <row r="8" spans="1:22" ht="23.25" customHeight="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="29">
+        <f>SUM(I$5:I7)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="29">
+        <f>SUM(J$5:J7)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="29">
+        <f>SUM(K$5:K7)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="29">
+        <f>SUM(L$5:L7)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="29">
+        <f>SUM(M$5:M7)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="29">
+        <f>SUM(N$5:N7)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="29">
+        <f>SUM(O$5:O7)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="29">
+        <f>SUM(P$5:P7)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="29">
+        <f>SUM(Q$5:Q7)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="29">
+        <f>SUM(R$5:R7)</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="29">
+        <f>SUM(S$5:S7)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="29">
+        <f>SUM(T$5:T7)</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="26"/>
+      <c r="V8" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:S1"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup orientation="landscape" scale="95" r:id="rId1"/>

</xml_diff>